<commit_message>
change time for auto export and mail daily income
</commit_message>
<xml_diff>
--- a/employee_data.xlsx
+++ b/employee_data.xlsx
@@ -12,7 +12,25 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Restaurant</t>
+  </si>
   <si>
     <t>Dao</t>
   </si>
@@ -149,7 +167,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -192,87 +210,107 @@
         <v>10</v>
       </c>
       <c r="F2" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F3" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F4" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F5" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F6" t="s">
-        <v>5</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>